<commit_message>
Patch + Final stage
</commit_message>
<xml_diff>
--- a/Rapports SEO/P4_01_Analyse.xlsx
+++ b/Rapports SEO/P4_01_Analyse.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Panzer\Desktop\Projet 4_Lenoir_Nicolas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD16D8E2-D4D9-4E2B-97C1-675B7F6B2509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A470F613-2DCD-4882-90EE-27259BBD49D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="16230" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
-    <sheet name="10 recommandations SEO" sheetId="6" r:id="rId2"/>
-    <sheet name="Check-list accessibilité mobile" sheetId="7" r:id="rId3"/>
+    <sheet name="Check-list accessibilité mobile" sheetId="7" r:id="rId2"/>
+    <sheet name="10 recommandations SEO" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="154">
   <si>
     <t>Catégorie</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>Ne jamais inclure du texte dans une image,préférez une description lisible par google et accessible par l'utilisateur via les balises &lt;alt&gt;, &lt;figure&gt; et &lt;figcaption&gt;.</t>
-  </si>
-  <si>
-    <t>Retirer le texte des images,et ajouter les balises &lt;alt&gt;,&lt;figure&gt; et &lt;figcaption&gt; pour décrire le contenu de celles-ci.</t>
   </si>
   <si>
     <t>Absence de balises sémantiques</t>
@@ -624,9 +621,6 @@
     <t>NOTE: je me suis permi d'ajouter + de 10 recommendations pour avoir un réel résultat d'optimisation</t>
   </si>
   <si>
-    <t>Balise meta &lt;description&gt; vide</t>
-  </si>
-  <si>
     <t>contenu ainsi que la quantité/qualité des mots clé insuffisants en gégénrale</t>
   </si>
   <si>
@@ -652,6 +646,33 @@
   </si>
   <si>
     <t>Si les balises meta ne sont pas exploités,alors les articles du site dans les réseaux sociaux ne seront pas ou mal diffusés…</t>
+  </si>
+  <si>
+    <t>Abscence d'attributs "defer" dans les balises &lt;script&gt;</t>
+  </si>
+  <si>
+    <t>L'abscence d'attributs "defer" dans &lt;script&gt; enlève un moyen d'optimiser la rapidité du temps de chargement des pages,"defer" pour charger le contenu une fois celui-ci téléchargé.</t>
+  </si>
+  <si>
+    <t>Si ces balises ne sont pas remplies correctement,google n'affichera pas de description dans la recherche</t>
+  </si>
+  <si>
+    <t>Balises meta &lt;description&gt; vide et title pas pertinente(.)</t>
+  </si>
+  <si>
+    <t>Toujours remplir ces balises pour que google affiche la decription dans les résultats de la recherche.</t>
+  </si>
+  <si>
+    <t>Remplir les balises meta descritpion et title.</t>
+  </si>
+  <si>
+    <t>Ajouter les balises sémantiques &lt;header&gt;,&lt;main&gt;,&lt;section&gt;&lt;article&gt;,&lt;footer&gt;…etc pour structurer le site .</t>
+  </si>
+  <si>
+    <t>Retirer les images avec du texte,ajouter une div et un paragraphe.Compléter les balises &lt;alt&gt; pour décrire le contenu des images si ce n'est pas déjà fait.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer la couleur du texte (plus claire) ou du fond en respectant au mieux la charte graphique du site et les règles du WCAG 2.0 </t>
   </si>
 </sst>
 </file>
@@ -1491,16 +1512,16 @@
       <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.27734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.27734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.0546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68" style="1" customWidth="1"/>
     <col min="4" max="4" width="89.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="74.0546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.38671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="74" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="11.27734375" style="1"/>
+    <col min="27" max="16384" width="11.21875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1564,21 +1585,21 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" ht="31.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>13</v>
@@ -1627,7 +1648,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26" ht="31.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
@@ -1719,7 +1740,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>40</v>
@@ -1746,14 +1767,14 @@
         <v>45</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26" ht="31.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>16</v>
       </c>
@@ -1774,7 +1795,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="62.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26" ht="62.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
@@ -1842,13 +1863,13 @@
         <v>32</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>62</v>
@@ -1858,7 +1879,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="63.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="63.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>16</v>
       </c>
@@ -1866,13 +1887,13 @@
         <v>63</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>139</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>13</v>
@@ -1884,37 +1905,37 @@
         <v>16</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="63" t="s">
-        <v>67</v>
-      </c>
       <c r="F18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="50.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="50.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="62" t="s">
         <v>107</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>108</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>13</v>
@@ -1926,16 +1947,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>13</v>
@@ -1947,37 +1968,37 @@
         <v>16</v>
       </c>
       <c r="B21" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="45" t="s">
-        <v>95</v>
-      </c>
       <c r="F21" s="41" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="32.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="32.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="E22" s="64" t="s">
         <v>103</v>
-      </c>
-      <c r="E22" s="64" t="s">
-        <v>104</v>
       </c>
       <c r="F22" s="42" t="s">
         <v>13</v>
@@ -1994,10 +2015,10 @@
     </row>
     <row r="24" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D24" s="66" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2008,975 +2029,975 @@
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="46" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="47" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="49" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="50" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="51" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="52" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="53" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="54" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="55" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="56" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="57" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="58" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="59" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="60" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="61" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="62" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="63" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="64" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="65" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="66" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="67" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="68" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="69" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="70" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="71" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="72" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="73" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="74" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="75" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="76" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="77" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="78" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="79" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="80" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="81" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="82" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="87" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="88" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="89" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="90" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="91" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="92" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="93" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="94" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="95" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="96" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="97" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="98" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="99" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="100" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="101" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="102" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="103" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="104" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="105" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="106" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="107" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="108" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="109" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="110" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="111" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="112" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="113" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="114" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="115" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="116" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="117" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="118" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="119" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="120" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="121" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="122" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="123" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="124" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="125" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="126" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="127" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="128" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="129" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="130" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="131" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="132" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="133" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="134" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="135" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="136" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="137" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="138" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="139" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="140" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="141" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="142" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="143" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="144" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="145" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="146" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="147" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="148" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="149" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="150" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="151" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="152" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="153" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="154" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="155" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="156" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="157" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="158" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="159" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="160" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="161" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="162" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="163" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="164" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="165" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="166" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="167" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="168" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="169" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="170" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="171" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="172" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="173" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="174" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="175" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="176" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="177" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="178" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="179" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="180" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="181" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="182" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="183" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="184" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="185" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="186" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="187" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="188" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="189" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="190" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="191" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="192" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="193" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="194" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="195" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="196" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="197" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="198" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="199" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="200" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="201" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="202" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="203" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="204" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="205" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="206" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="207" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="208" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="209" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="210" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="211" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="212" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="213" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="214" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="215" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="216" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="217" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="218" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="219" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="220" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="221" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="222" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="223" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="224" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="225" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="226" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="227" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="228" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="229" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="230" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="231" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="232" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="233" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="234" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="235" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="236" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="237" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="238" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="239" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="240" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="241" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="242" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="243" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="244" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="245" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="246" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="247" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="248" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="249" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="250" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="251" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="252" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="253" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="254" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="255" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="256" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="257" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="258" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="259" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="260" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="261" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="262" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="263" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="264" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="265" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="266" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="267" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="268" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="269" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="270" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="271" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="272" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="273" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="274" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="275" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="276" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="277" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="278" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="279" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="280" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="281" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="282" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="283" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="284" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="285" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="286" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="287" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="288" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="289" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="290" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="291" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="292" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="293" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="294" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="295" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="296" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="297" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="298" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="299" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="300" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="301" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="302" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="303" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="304" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="305" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="306" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="307" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="308" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="309" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="310" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="311" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="312" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="313" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="314" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="315" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="316" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="317" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="318" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="319" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="320" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="321" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="322" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="323" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="324" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="325" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="326" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="327" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="328" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="329" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="330" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="331" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="332" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="333" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="334" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="335" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="336" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="337" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="338" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="339" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="340" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="341" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="342" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="343" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="344" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="345" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="346" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="347" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="348" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="349" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="350" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="351" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="352" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="353" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="354" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="355" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="356" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="357" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="358" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="359" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="360" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="361" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="362" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="363" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="364" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="365" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="366" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="367" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="368" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="369" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="370" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="371" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="372" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="373" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="374" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="375" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="376" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="377" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="378" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="379" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="380" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="381" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="382" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="383" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="384" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="385" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="386" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="387" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="388" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="389" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="390" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="391" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="392" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="393" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="394" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="395" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="396" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="397" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="398" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="399" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="400" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="401" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="402" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="403" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="404" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="405" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="406" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="407" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="408" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="409" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="410" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="411" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="412" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="413" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="414" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="415" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="416" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="417" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="418" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="419" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="420" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="421" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="422" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="423" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="424" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="425" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="426" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="427" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="428" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="429" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="430" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="431" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="432" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="433" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="434" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="435" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="436" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="437" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="438" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="439" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="440" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="441" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="442" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="443" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="444" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="445" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="446" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="447" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="448" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="449" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="450" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="451" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="452" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="453" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="454" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="455" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="456" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="457" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="458" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="459" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="460" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="461" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="462" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="463" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="464" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="465" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="466" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="467" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="468" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="469" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="470" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="471" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="472" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="473" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="474" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="475" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="476" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="477" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="478" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="479" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="480" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="481" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="482" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="483" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="484" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="485" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="486" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="487" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="488" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="489" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="490" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="491" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="492" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="493" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="494" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="495" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="496" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="497" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="498" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="499" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="500" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="501" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="502" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="503" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="504" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="505" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="506" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="507" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="508" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="509" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="510" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="511" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="512" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="513" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="514" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="515" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="516" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="517" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="518" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="519" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="520" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="521" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="522" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="523" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="524" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="525" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="526" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="527" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="528" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="529" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="530" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="531" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="532" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="533" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="534" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="535" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="536" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="537" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="538" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="539" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="540" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="541" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="542" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="543" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="544" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="545" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="546" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="547" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="548" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="549" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="550" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="551" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="552" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="553" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="554" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="555" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="556" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="557" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="558" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="559" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="560" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="561" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="562" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="563" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="564" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="565" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="566" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="567" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="568" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="569" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="570" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="571" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="572" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="573" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="574" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="575" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="576" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="577" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="578" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="579" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="580" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="581" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="582" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="583" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="584" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="585" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="586" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="587" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="588" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="589" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="590" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="591" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="592" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="593" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="594" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="595" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="596" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="597" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="598" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="599" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="600" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="601" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="602" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="603" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="604" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="605" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="606" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="607" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="608" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="609" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="610" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="611" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="612" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="613" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="614" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="615" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="616" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="617" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="618" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="619" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="620" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="621" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="622" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="623" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="624" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="625" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="626" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="627" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="628" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="629" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="630" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="631" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="632" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="633" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="634" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="635" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="636" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="637" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="638" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="639" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="640" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="641" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="642" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="643" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="644" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="645" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="646" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="647" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="648" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="649" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="650" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="651" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="652" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="653" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="654" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="655" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="656" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="657" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="658" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="659" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="660" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="661" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="662" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="663" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="664" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="665" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="666" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="667" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="668" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="669" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="670" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="671" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="672" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="673" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="674" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="675" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="676" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="677" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="678" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="679" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="680" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="681" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="682" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="683" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="684" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="685" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="686" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="687" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="688" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="689" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="690" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="691" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="692" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="693" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="694" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="695" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="696" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="697" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="698" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="699" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="700" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="701" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="702" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="703" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="704" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="705" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="706" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="707" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="708" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="709" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="710" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="711" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="712" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="713" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="714" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="715" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="716" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="717" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="718" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="719" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="720" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="721" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="722" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="723" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="724" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="725" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="726" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="727" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="728" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="729" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="730" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="731" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="732" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="733" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="734" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="735" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="736" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="737" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="738" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="739" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="740" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="741" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="742" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="743" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="744" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="745" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="746" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="747" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="748" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="749" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="750" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="751" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="752" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="753" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="754" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="755" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="756" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="757" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="758" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="759" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="760" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="761" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="762" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="763" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="764" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="765" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="766" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="767" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="768" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="769" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="770" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="771" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="772" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="773" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="774" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="775" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="776" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="777" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="778" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="779" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="780" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="781" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="782" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="783" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="784" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="785" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="786" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="787" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="788" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="789" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="790" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="791" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="792" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="793" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="794" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="795" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="796" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="797" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="798" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="799" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="800" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="801" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="802" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="803" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="804" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="805" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="806" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="807" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="808" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="809" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="810" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="811" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="812" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="813" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="814" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="815" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="816" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="817" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="818" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="819" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="820" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="821" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="822" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="823" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="824" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="825" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="826" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="827" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="828" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="829" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="830" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="831" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="832" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="833" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="834" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="835" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="836" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="837" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="838" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="839" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="840" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="841" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="842" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="843" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="844" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="845" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="846" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="847" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="848" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="849" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="850" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="851" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="852" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="853" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="854" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="855" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="856" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="857" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="858" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="859" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="860" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="861" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="862" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="863" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="864" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="865" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="866" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="867" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="868" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="869" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="870" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="871" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="872" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="873" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="874" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="875" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="876" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="877" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="878" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="879" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="880" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="881" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="882" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="883" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="884" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="885" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="886" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="887" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="888" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="889" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="890" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="891" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="892" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="893" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="894" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="895" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="896" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="897" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="898" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="899" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="900" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="901" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="902" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="903" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="904" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="905" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="906" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="907" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="908" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="909" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="910" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="911" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="912" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="913" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="914" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="915" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="916" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="917" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="918" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="919" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="920" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="921" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="922" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="923" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="924" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="925" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="926" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="927" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="928" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="929" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="930" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="931" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="932" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="933" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="934" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="935" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="936" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="937" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="938" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="939" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="940" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="941" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="942" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="943" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="944" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="945" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="946" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="947" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="948" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="949" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="950" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="951" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="952" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="953" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="954" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="955" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="956" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="957" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="958" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="959" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="960" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="961" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="962" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="963" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="964" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="965" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="966" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="967" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="968" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="969" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="970" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="971" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="972" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="973" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="974" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="975" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="976" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="977" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="978" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="979" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="980" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="981" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="982" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="983" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="984" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="985" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="986" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="987" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="988" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="989" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="990" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="991" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="992" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="993" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="994" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="995" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="996" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="997" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="998" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="999" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="1000" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="1001" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{ABF0E76D-1119-49BB-B493-DED7DBC05376}"/>
@@ -3007,27 +3028,184 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37237595-47C7-411C-9286-2F7286EF84D7}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" customWidth="1"/>
+    <col min="4" max="4" width="44.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+    </row>
+    <row r="2" spans="1:6" ht="45.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="54"/>
+      <c r="F2" s="52"/>
+    </row>
+    <row r="3" spans="1:6" ht="60.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="55"/>
+      <c r="F3" s="53"/>
+    </row>
+    <row r="4" spans="1:6" ht="30.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="56"/>
+      <c r="F4" s="52"/>
+    </row>
+    <row r="5" spans="1:6" ht="90.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="55"/>
+      <c r="F5" s="53"/>
+    </row>
+    <row r="6" spans="1:6" ht="90.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="56"/>
+      <c r="F6" s="52"/>
+    </row>
+    <row r="7" spans="1:6" ht="60.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="56"/>
+      <c r="F7" s="52"/>
+    </row>
+    <row r="8" spans="1:6" ht="45.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="56"/>
+      <c r="F8" s="52"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E9" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C13" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60247581-3164-4DD6-8EF8-CBFC2A4B2B97}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
     <col min="2" max="2" width="32.44140625" customWidth="1"/>
     <col min="3" max="3" width="50.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
+    <col min="5" max="5" width="30.44140625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -3036,10 +3214,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>5</v>
@@ -3068,16 +3246,16 @@
     <row r="2" spans="1:26" s="1" customFormat="1" ht="67.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
       <c r="B2" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>13</v>
@@ -3086,10 +3264,10 @@
     </row>
     <row r="3" spans="1:26" s="1" customFormat="1" ht="67.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>19</v>
@@ -3108,7 +3286,7 @@
     <row r="4" spans="1:26" s="1" customFormat="1" ht="67.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="27"/>
       <c r="B4" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>55</v>
@@ -3117,7 +3295,7 @@
         <v>57</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>13</v>
@@ -3145,7 +3323,7 @@
     </row>
     <row r="6" spans="1:26" s="1" customFormat="1" ht="82.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>50</v>
@@ -3167,15 +3345,15 @@
     <row r="7" spans="1:26" s="1" customFormat="1" ht="82.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="21"/>
       <c r="B7" s="23" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="C7" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F7" s="24" t="s">
@@ -3204,7 +3382,7 @@
     </row>
     <row r="9" spans="1:26" s="1" customFormat="1" ht="67.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>43</v>
@@ -3213,10 +3391,10 @@
         <v>44</v>
       </c>
       <c r="D9" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="62" t="s">
         <v>83</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>84</v>
       </c>
       <c r="F9" s="26" t="s">
         <v>13</v>
@@ -3226,16 +3404,16 @@
     <row r="10" spans="1:26" s="1" customFormat="1" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="27"/>
       <c r="B10" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="F10" s="18" t="s">
         <v>13</v>
@@ -3245,16 +3423,16 @@
     <row r="11" spans="1:26" s="1" customFormat="1" ht="33.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="70"/>
       <c r="B11" s="71" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C11" s="72" t="s">
-        <v>12</v>
+        <v>147</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="72" t="s">
-        <v>10</v>
+        <v>149</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>150</v>
       </c>
       <c r="F11" s="73" t="s">
         <v>13</v>
@@ -3263,13 +3441,13 @@
     </row>
     <row r="12" spans="1:26" s="1" customFormat="1" ht="82.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>40</v>
@@ -3293,7 +3471,7 @@
       <c r="D13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="24" t="s">
@@ -3303,19 +3481,19 @@
     </row>
     <row r="14" spans="1:26" s="1" customFormat="1" ht="91.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>65</v>
+      <c r="E14" s="63" t="s">
+        <v>152</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>13</v>
@@ -3325,16 +3503,16 @@
     <row r="15" spans="1:26" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="27"/>
       <c r="B15" s="33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>13</v>
@@ -3342,7 +3520,7 @@
     </row>
     <row r="16" spans="1:26" s="1" customFormat="1" ht="82.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>47</v>
@@ -3367,13 +3545,13 @@
         <v>63</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F17" s="36" t="s">
         <v>13</v>
@@ -3381,7 +3559,7 @@
     </row>
     <row r="18" spans="1:7" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>30</v>
@@ -3401,18 +3579,18 @@
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="82.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="62" t="s">
         <v>61</v>
       </c>
       <c r="F19" s="24" t="s">
@@ -3422,19 +3600,19 @@
     </row>
     <row r="20" spans="1:7" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="69" t="s">
         <v>103</v>
-      </c>
-      <c r="E20" s="69" t="s">
-        <v>104</v>
       </c>
       <c r="F20" s="38" t="s">
         <v>13</v>
@@ -3442,19 +3620,19 @@
     </row>
     <row r="21" spans="1:7" ht="90.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>13</v>
@@ -3462,21 +3640,21 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E23" s="68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D25" s="75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E25" s="76"/>
       <c r="F25" s="77"/>
@@ -3511,161 +3689,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId22"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37237595-47C7-411C-9286-2F7286EF84D7}">
-  <dimension ref="A1:F13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1"/>
-    <col min="3" max="3" width="50.44140625" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-    </row>
-    <row r="2" spans="1:6" ht="45.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="52"/>
-    </row>
-    <row r="3" spans="1:6" ht="60.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="53"/>
-    </row>
-    <row r="4" spans="1:6" ht="30.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="61" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="56"/>
-      <c r="F4" s="52"/>
-    </row>
-    <row r="5" spans="1:6" ht="90.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="57" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="53"/>
-    </row>
-    <row r="6" spans="1:6" ht="90.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="57" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="52"/>
-    </row>
-    <row r="7" spans="1:6" ht="60.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="57" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="52"/>
-    </row>
-    <row r="8" spans="1:6" ht="45.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="E8" s="56"/>
-      <c r="F8" s="52"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="E9" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C13" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>